<commit_message>
Continued update of nomenclature and identified new issues
Updated nomenclature for naming files/variables in readme

Identified new issues in the running of Saved Filters
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/Extended_Attributes.xlsx
+++ b/utils/config/ReferenceLists/Extended_Attributes.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{C5FDE849-DB08-43CB-B737-4F655FEFE0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C1C0B91-67AF-44BF-A89C-FB9CC4A4507C}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{C5FDE849-DB08-43CB-B737-4F655FEFE0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5B21300-CEE2-4074-835A-46AA566032C4}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{37C43DCA-9008-43E6-91C9-4FE49E69DD6A}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{37C43DCA-9008-43E6-91C9-4FE49E69DD6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Extended_Attributes" sheetId="1" r:id="rId1"/>
-    <sheet name="DropdownLists" sheetId="2" r:id="rId2"/>
+    <sheet name="Dropdownlists" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1556,7 +1556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFA14A41-9107-421E-8224-801D8144DA01}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2126,7 +2126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F259C135-316D-4E6D-99E9-298DC78EB6DB}">
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>